<commit_message>
add case1 case2 bookingFromExcel and bookingWithoutLogin
</commit_message>
<xml_diff>
--- a/src/test/resources/BookingData.xlsx
+++ b/src/test/resources/BookingData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JAVA project\Testing05_Nhom2\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JAVA project\Testing05_Nhom2\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49D1299-8513-4EF3-9830-59816F546950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3DCCE8-E2C9-4F7A-86CB-77C13A0704B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C03C9B1-B188-402C-8949-FC84BB5B4FF3}"/>
+    <workbookView xWindow="5052" yWindow="3744" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{0C03C9B1-B188-402C-8949-FC84BB5B4FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="data1" sheetId="1" r:id="rId1"/>
+    <sheet name="data2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Email</t>
   </si>
@@ -52,6 +53,18 @@
   </si>
   <si>
     <t>Phòng mùa hè</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Địa điểm </t>
+  </si>
+  <si>
+    <t>Nhận phòng</t>
+  </si>
+  <si>
+    <t>Trả phòng</t>
+  </si>
+  <si>
+    <t>Số khách</t>
   </si>
 </sst>
 </file>
@@ -98,12 +111,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -421,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E40D1DE-244C-42B8-97ED-ADAED0432D20}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -474,4 +488,58 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6A08C5-A6AA-4549-896C-57F5EF282D7D}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.796875" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="16.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45931</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45945</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modify file and add testcase 345678
</commit_message>
<xml_diff>
--- a/src/test/resources/BookingData.xlsx
+++ b/src/test/resources/BookingData.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JAVA project\Testing05_Nhom2\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JAVA project\Testing05_Nhom2\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3DCCE8-E2C9-4F7A-86CB-77C13A0704B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49D1299-8513-4EF3-9830-59816F546950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5052" yWindow="3744" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{0C03C9B1-B188-402C-8949-FC84BB5B4FF3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C03C9B1-B188-402C-8949-FC84BB5B4FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="data1" sheetId="1" r:id="rId1"/>
-    <sheet name="data2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Email</t>
   </si>
@@ -53,18 +52,6 @@
   </si>
   <si>
     <t>Phòng mùa hè</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Địa điểm </t>
-  </si>
-  <si>
-    <t>Nhận phòng</t>
-  </si>
-  <si>
-    <t>Trả phòng</t>
-  </si>
-  <si>
-    <t>Số khách</t>
   </si>
 </sst>
 </file>
@@ -111,13 +98,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -435,7 +421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E40D1DE-244C-42B8-97ED-ADAED0432D20}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -488,58 +474,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6A08C5-A6AA-4549-896C-57F5EF282D7D}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.796875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="16.296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3">
-        <v>45931</v>
-      </c>
-      <c r="D2" s="3">
-        <v>45945</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>